<commit_message>
shortened exhibit names and item descriptions
</commit_message>
<xml_diff>
--- a/Hard_Props_Pull_Schedule.xlsx
+++ b/Hard_Props_Pull_Schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JHighsmith\GitHub\sked\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D39CE050-71F4-4115-B1DE-CD1D68EEBC21}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F505C984-1E7D-4E45-8EA1-022BBDE78892}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="330" yWindow="90" windowWidth="26250" windowHeight="15405" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="98">
   <si>
     <t>Area</t>
   </si>
@@ -77,9 +77,6 @@
     <t>Light Table Pieces</t>
   </si>
   <si>
-    <t>Sensory Table Pieces (if hard plastic)</t>
-  </si>
-  <si>
     <t>Kitchen</t>
   </si>
   <si>
@@ -152,9 +149,6 @@
     <t>Milking bottles</t>
   </si>
   <si>
-    <t>Mini Farm Animals from barn table</t>
-  </si>
-  <si>
     <t>Pollys</t>
   </si>
   <si>
@@ -188,9 +182,6 @@
     <t>Pizza Pans</t>
   </si>
   <si>
-    <t>Hit the Trail</t>
-  </si>
-  <si>
     <t>Blue dishes</t>
   </si>
   <si>
@@ -239,36 +230,21 @@
     <t>Salad Spinner bowls</t>
   </si>
   <si>
-    <t>STEMosphere</t>
-  </si>
-  <si>
     <t>Duplo/Lego Bricks</t>
   </si>
   <si>
     <t>Tower Discs</t>
   </si>
   <si>
-    <t>Magnet building toys &amp; balls</t>
-  </si>
-  <si>
     <t>Go Zone</t>
   </si>
   <si>
     <t>Kinnex pieces</t>
   </si>
   <si>
-    <t xml:space="preserve"> Friday</t>
-  </si>
-  <si>
     <t>Custom</t>
   </si>
   <si>
-    <t>Around Town</t>
-  </si>
-  <si>
-    <t>Moneypalooza</t>
-  </si>
-  <si>
     <t>Campfire</t>
   </si>
   <si>
@@ -314,12 +290,6 @@
     <t>Splash</t>
   </si>
   <si>
-    <t>Power2Play</t>
-  </si>
-  <si>
-    <t>IdeaWorks</t>
-  </si>
-  <si>
     <t>Gallery</t>
   </si>
   <si>
@@ -327,6 +297,33 @@
   </si>
   <si>
     <t>Tray</t>
+  </si>
+  <si>
+    <t>Mini Barm Animals</t>
+  </si>
+  <si>
+    <t>Magnet building toys</t>
+  </si>
+  <si>
+    <t>Hard Sensory Bin Items</t>
+  </si>
+  <si>
+    <t>IW</t>
+  </si>
+  <si>
+    <t>P2P</t>
+  </si>
+  <si>
+    <t>STEMo</t>
+  </si>
+  <si>
+    <t>AT</t>
+  </si>
+  <si>
+    <t>HTT</t>
+  </si>
+  <si>
+    <t>MP</t>
   </si>
 </sst>
 </file>
@@ -495,7 +492,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -509,9 +506,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -522,6 +520,15 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -744,6 +751,9 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{37147807-599D-4AC4-8D71-F997FEFD3F07}" name="Table1" displayName="Table1" ref="A1:E58" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
   <autoFilter ref="A1:E58" xr:uid="{7DBD9A50-CA46-40A4-9598-FE2CE577E5CE}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E58">
+    <sortCondition ref="D1:D58"/>
+  </sortState>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{E67CD828-10A4-4F13-B4D5-FA0822CDA957}" name="Gallery" dataDxfId="5"/>
     <tableColumn id="2" xr3:uid="{87987B2D-BD9D-49C3-AB0D-727566FF9C4D}" name="Area"/>
@@ -1055,269 +1065,265 @@
   <dimension ref="A1:E58"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="A52" sqref="A52:A58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.140625" style="5" customWidth="1"/>
-    <col min="2" max="2" width="24.28515625" style="5" customWidth="1"/>
-    <col min="3" max="3" width="51.5703125" style="5" customWidth="1"/>
-    <col min="4" max="4" width="19" style="5" customWidth="1"/>
-    <col min="5" max="5" width="26.140625" style="5" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="5"/>
+    <col min="1" max="1" width="11" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
-        <v>96</v>
-      </c>
-      <c r="B1" s="10" t="s">
+      <c r="A1" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="B1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="11" t="s">
-        <v>97</v>
-      </c>
-      <c r="D1" s="11" t="s">
+      <c r="C1" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="D1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="11" t="s">
-        <v>98</v>
+      <c r="E1" s="10" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="B3" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2" s="2" t="s">
+      <c r="C3" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="E3" s="15" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+    <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="B4" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+      <c r="C4" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="D4" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="E4" s="15" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="B5" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>7</v>
+      <c r="C5" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="D5" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="E5" s="15" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E6" s="2" t="s">
+      <c r="A6" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="C6" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="D6" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="E6" s="15" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E7" s="2" t="s">
+      <c r="A7" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="D7" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="E7" s="15" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
-        <v>77</v>
+      <c r="A8" s="6" t="s">
+        <v>57</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>13</v>
+        <v>57</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>14</v>
+        <v>58</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>4</v>
+        <v>61</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
-        <v>77</v>
+      <c r="A9" s="6" t="s">
+        <v>93</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>13</v>
+        <v>59</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>15</v>
+        <v>60</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>4</v>
+        <v>61</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
-        <v>77</v>
+      <c r="A10" s="6" t="s">
+        <v>93</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>16</v>
+        <v>59</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>17</v>
+        <v>62</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>4</v>
+        <v>61</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
-        <v>77</v>
+      <c r="A11" s="6" t="s">
+        <v>93</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>16</v>
+        <v>59</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>18</v>
+        <v>63</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>4</v>
+        <v>61</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
-        <v>77</v>
+      <c r="A12" s="6" t="s">
+        <v>93</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>16</v>
+        <v>59</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>19</v>
+        <v>64</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>4</v>
+        <v>61</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
-        <v>77</v>
+      <c r="A13" s="6" t="s">
+        <v>93</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>16</v>
+        <v>59</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>20</v>
+        <v>65</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>4</v>
+        <v>61</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>16</v>
-      </c>
+        <v>94</v>
+      </c>
+      <c r="B14" s="11"/>
       <c r="C14" s="2" t="s">
-        <v>21</v>
+        <v>66</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>4</v>
+        <v>61</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>7</v>
+        <v>70</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>16</v>
-      </c>
+        <v>94</v>
+      </c>
+      <c r="B15" s="1"/>
       <c r="C15" s="2" t="s">
-        <v>22</v>
+        <v>67</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>4</v>
+        <v>61</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>7</v>
@@ -1325,594 +1331,592 @@
     </row>
     <row r="16" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="B16" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B16" s="1"/>
+      <c r="C16" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A20" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A22" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A23" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A24" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A25" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C25" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="D25" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A26" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A27" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A28" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A29" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A30" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A31" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A32" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C32" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D16" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C17" s="2" t="s">
+      <c r="D32" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A33" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C33" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D17" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C18" s="2" t="s">
+      <c r="D33" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A34" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C34" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D18" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C19" s="2" t="s">
+      <c r="D34" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A35" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="B35" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D19" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="B20" s="1" t="s">
+      <c r="C35" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="D35" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A36" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C36" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D20" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C21" s="2" t="s">
+      <c r="D36" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A37" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C37" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D21" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C22" s="2" t="s">
+      <c r="D37" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A38" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C38" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D22" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C23" s="2" t="s">
+      <c r="D38" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A39" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="B39" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D23" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A24" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="B24" s="1" t="s">
+      <c r="C39" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C24" s="2" t="s">
+      <c r="D39" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A40" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="B40" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="D24" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="B25" s="1" t="s">
+      <c r="C40" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C25" s="2" t="s">
+      <c r="D40" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A41" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C41" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="D25" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A26" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C26" s="2" t="s">
+      <c r="D41" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A42" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C42" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D26" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E26" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A27" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C27" s="2" t="s">
+      <c r="D42" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A43" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C43" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D27" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E27" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A28" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C28" s="2" t="s">
+      <c r="D43" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A44" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="B44" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C44" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="D28" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E28" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A29" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E29" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A30" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E30" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A31" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="E31" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A32" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D32" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="E32" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A33" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="D33" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="E33" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A34" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="E34" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A35" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="E35" s="2" t="s">
+      <c r="D44" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="E44" s="13" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A45" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="B45" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C45" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="D45" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="E45" s="13" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A46" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="B46" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="C46" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="D46" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="E46" s="13" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A36" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="E36" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A37" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="C37" s="2" t="s">
+    <row r="47" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A47" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="B47" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="C47" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="D47" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="D37" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="E37" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A38" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="D38" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="E38" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A39" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="D39" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="E39" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A40" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="B40" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="D40" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="E40" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A41" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="D41" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="E41" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A42" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="D42" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="E42" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A43" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="C43" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="D43" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="E43" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A44" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="B44" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="C44" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="D44" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="E44" s="6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A45" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="B45" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="C45" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="D45" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="E45" s="6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A46" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="B46" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="C46" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="D46" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="E46" s="6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A47" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="B47" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="C47" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="D47" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="E47" s="6" t="s">
+      <c r="E47" s="13" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="48" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="B48" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="C48" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="D48" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="E48" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="B48" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="C48" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="D48" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="E48" s="13" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="49" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A49" s="5" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>60</v>
+        <v>73</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="50" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A50" s="5" t="s">
-        <v>94</v>
+        <v>53</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>62</v>
+        <v>74</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="D50" s="4" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="E50" s="4" t="s">
         <v>7</v>
@@ -1920,132 +1924,138 @@
     </row>
     <row r="51" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A51" s="5" t="s">
-        <v>94</v>
+        <v>53</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>62</v>
+        <v>75</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>65</v>
+        <v>76</v>
       </c>
       <c r="D51" s="4" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="E51" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A52" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C52" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D52" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="E52" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A53" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C53" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D53" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="E53" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A54" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C54" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D54" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="E54" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A55" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="B55" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="C55" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D55" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="E55" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A56" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C56" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D56" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="E56" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="52" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A52" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="B52" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="C52" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="D52" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="E52" s="4" t="s">
+    <row r="57" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A57" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="B57" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C57" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D57" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="E57" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="53" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A53" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="B53" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="C53" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="D53" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="E53" s="4" t="s">
+    <row r="58" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A58" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D58" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E58" s="2" t="s">
         <v>5</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A54" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="B54" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="C54" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="D54" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="E54" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A55" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="B55" s="7"/>
-      <c r="C55" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="D55" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="E55" s="4" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A56" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="B56" s="3"/>
-      <c r="C56" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="D56" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="E56" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A57" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="B57" s="3"/>
-      <c r="C57" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="D57" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="E57" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A58" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="B58" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="C58" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="D58" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="E58" s="2" t="s">
-        <v>76</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added hard-prop pulls, split weekend
</commit_message>
<xml_diff>
--- a/Hard_Props_Pull_Schedule.xlsx
+++ b/Hard_Props_Pull_Schedule.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JHighsmith\GitHub\sked\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B772461B-307D-490E-A1C4-E969C38D0644}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D2EC0C0-366D-4627-978F-EF663B2B1CED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="330" yWindow="90" windowWidth="26250" windowHeight="15405" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -293,9 +293,6 @@
     <t>Tray</t>
   </si>
   <si>
-    <t>Mini Barm Animals</t>
-  </si>
-  <si>
     <t>Magnet building toys</t>
   </si>
   <si>
@@ -324,6 +321,9 @@
   </si>
   <si>
     <t>Hard Sensory Items</t>
+  </si>
+  <si>
+    <t>Mini Farm Animals</t>
   </si>
 </sst>
 </file>
@@ -520,57 +520,6 @@
   <dxfs count="6">
     <dxf>
       <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="0"/>
-        <name val="Gilroy"/>
-        <family val="3"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <name val="Gilroy"/>
-        <family val="3"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -719,6 +668,57 @@
         <horizontal/>
       </border>
     </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <name val="Gilroy"/>
+        <family val="3"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="0"/>
+        <name val="Gilroy"/>
+        <family val="3"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
@@ -733,17 +733,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{37147807-599D-4AC4-8D71-F997FEFD3F07}" name="Table1" displayName="Table1" ref="A1:E58" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{37147807-599D-4AC4-8D71-F997FEFD3F07}" name="Table1" displayName="Table1" ref="A1:E58" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
   <autoFilter ref="A1:E58" xr:uid="{7DBD9A50-CA46-40A4-9598-FE2CE577E5CE}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E58">
     <sortCondition ref="D1:D58"/>
   </sortState>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{E67CD828-10A4-4F13-B4D5-FA0822CDA957}" name="Gallery" dataDxfId="5"/>
+    <tableColumn id="1" xr3:uid="{E67CD828-10A4-4F13-B4D5-FA0822CDA957}" name="Gallery" dataDxfId="3"/>
     <tableColumn id="2" xr3:uid="{87987B2D-BD9D-49C3-AB0D-727566FF9C4D}" name="Area"/>
-    <tableColumn id="3" xr3:uid="{67792699-C3EA-4BEA-AC3B-09176DFE3712}" name="Item" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{59F296FE-5EED-41DB-9FE4-E8B4143F0B64}" name="Day" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{76A8B66D-952F-4731-AFB5-0DD663D56ECE}" name="Tray" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{67792699-C3EA-4BEA-AC3B-09176DFE3712}" name="Item" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{59F296FE-5EED-41DB-9FE4-E8B4143F0B64}" name="Day" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{76A8B66D-952F-4731-AFB5-0DD663D56ECE}" name="Tray" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1048,8 +1048,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E58"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1081,7 +1081,7 @@
     </row>
     <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>66</v>
@@ -1200,7 +1200,7 @@
     </row>
     <row r="9" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>57</v>
@@ -1217,7 +1217,7 @@
     </row>
     <row r="10" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>57</v>
@@ -1234,7 +1234,7 @@
     </row>
     <row r="11" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>57</v>
@@ -1251,7 +1251,7 @@
     </row>
     <row r="12" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>57</v>
@@ -1268,7 +1268,7 @@
     </row>
     <row r="13" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>57</v>
@@ -1285,7 +1285,7 @@
     </row>
     <row r="14" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B14" s="11"/>
       <c r="C14" s="2" t="s">
@@ -1300,7 +1300,7 @@
     </row>
     <row r="15" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B15" s="1"/>
       <c r="C15" s="2" t="s">
@@ -1315,11 +1315,11 @@
     </row>
     <row r="16" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B16" s="1"/>
       <c r="C16" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>59</v>
@@ -1330,7 +1330,7 @@
     </row>
     <row r="17" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>2</v>
@@ -1347,7 +1347,7 @@
     </row>
     <row r="18" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>2</v>
@@ -1364,7 +1364,7 @@
     </row>
     <row r="19" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>2</v>
@@ -1381,7 +1381,7 @@
     </row>
     <row r="20" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>2</v>
@@ -1398,7 +1398,7 @@
     </row>
     <row r="21" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>10</v>
@@ -1415,7 +1415,7 @@
     </row>
     <row r="22" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>10</v>
@@ -1432,7 +1432,7 @@
     </row>
     <row r="23" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>13</v>
@@ -1449,13 +1449,13 @@
     </row>
     <row r="24" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>4</v>
@@ -1466,7 +1466,7 @@
     </row>
     <row r="25" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>15</v>
@@ -1483,7 +1483,7 @@
     </row>
     <row r="26" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>15</v>
@@ -1500,7 +1500,7 @@
     </row>
     <row r="27" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>15</v>
@@ -1517,7 +1517,7 @@
     </row>
     <row r="28" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>15</v>
@@ -1534,7 +1534,7 @@
     </row>
     <row r="29" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>15</v>
@@ -1551,7 +1551,7 @@
     </row>
     <row r="30" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>15</v>
@@ -1568,7 +1568,7 @@
     </row>
     <row r="31" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>15</v>
@@ -1585,7 +1585,7 @@
     </row>
     <row r="32" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>15</v>
@@ -1602,13 +1602,13 @@
     </row>
     <row r="33" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D33" s="2" t="s">
         <v>4</v>
@@ -1619,7 +1619,7 @@
     </row>
     <row r="34" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>15</v>
@@ -1636,7 +1636,7 @@
     </row>
     <row r="35" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>25</v>
@@ -1653,7 +1653,7 @@
     </row>
     <row r="36" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>25</v>
@@ -1670,7 +1670,7 @@
     </row>
     <row r="37" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>25</v>
@@ -1687,7 +1687,7 @@
     </row>
     <row r="38" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>25</v>
@@ -1704,7 +1704,7 @@
     </row>
     <row r="39" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A39" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>30</v>
@@ -1721,7 +1721,7 @@
     </row>
     <row r="40" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A40" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B40" s="7" t="s">
         <v>32</v>
@@ -1738,7 +1738,7 @@
     </row>
     <row r="41" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A41" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>32</v>
@@ -1755,7 +1755,7 @@
     </row>
     <row r="42" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A42" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>32</v>
@@ -1772,7 +1772,7 @@
     </row>
     <row r="43" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A43" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>32</v>
@@ -1789,7 +1789,7 @@
     </row>
     <row r="44" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A44" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B44" s="13" t="s">
         <v>32</v>
@@ -1806,13 +1806,13 @@
     </row>
     <row r="45" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A45" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B45" s="13" t="s">
         <v>32</v>
       </c>
       <c r="C45" s="13" t="s">
-        <v>87</v>
+        <v>97</v>
       </c>
       <c r="D45" s="13" t="s">
         <v>4</v>
@@ -1823,7 +1823,7 @@
     </row>
     <row r="46" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A46" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B46" s="13" t="s">
         <v>69</v>
@@ -1840,7 +1840,7 @@
     </row>
     <row r="47" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A47" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B47" s="13" t="s">
         <v>69</v>
@@ -1925,7 +1925,7 @@
     </row>
     <row r="52" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A52" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B52" s="3" t="s">
         <v>38</v>
@@ -1942,7 +1942,7 @@
     </row>
     <row r="53" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A53" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B53" s="3" t="s">
         <v>38</v>
@@ -1959,10 +1959,10 @@
     </row>
     <row r="54" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A54" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="B54" s="3" t="s">
         <v>94</v>
-      </c>
-      <c r="B54" s="3" t="s">
-        <v>95</v>
       </c>
       <c r="C54" s="4" t="s">
         <v>42</v>
@@ -1976,10 +1976,10 @@
     </row>
     <row r="55" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A55" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="B55" s="3" t="s">
         <v>94</v>
-      </c>
-      <c r="B55" s="3" t="s">
-        <v>95</v>
       </c>
       <c r="C55" s="4" t="s">
         <v>43</v>
@@ -1993,10 +1993,10 @@
     </row>
     <row r="56" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A56" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="B56" s="3" t="s">
         <v>94</v>
-      </c>
-      <c r="B56" s="3" t="s">
-        <v>95</v>
       </c>
       <c r="C56" s="4" t="s">
         <v>44</v>
@@ -2010,10 +2010,10 @@
     </row>
     <row r="57" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A57" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="B57" s="3" t="s">
         <v>94</v>
-      </c>
-      <c r="B57" s="3" t="s">
-        <v>95</v>
       </c>
       <c r="C57" s="4" t="s">
         <v>45</v>
@@ -2027,7 +2027,7 @@
     </row>
     <row r="58" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A58" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B58" s="1" t="s">
         <v>46</v>
@@ -2263,18 +2263,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2297,14 +2297,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D3F89562-4375-42AC-80C2-C5E69D9A52EC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{53E59BFD-F243-4730-8E2F-243A7D3E57EE}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="95d5ab19-5df0-4393-9a78-50cfb5c04389"/>
@@ -2319,4 +2311,12 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D3F89562-4375-42AC-80C2-C5E69D9A52EC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
added herb and carts pages, updated schedule for 1-16
</commit_message>
<xml_diff>
--- a/Hard_Props_Pull_Schedule.xlsx
+++ b/Hard_Props_Pull_Schedule.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JHighsmith\GitHub\sked\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D2EC0C0-366D-4627-978F-EF663B2B1CED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19C8F579-F675-4DCB-A926-2CAC4E8A5C2A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -44,9 +44,6 @@
     <t>Food Bowls</t>
   </si>
   <si>
-    <t>Sunday</t>
-  </si>
-  <si>
     <t>Pronged</t>
   </si>
   <si>
@@ -324,6 +321,9 @@
   </si>
   <si>
     <t>Mini Farm Animals</t>
+  </si>
+  <si>
+    <t>Monday</t>
   </si>
 </sst>
 </file>
@@ -1048,7 +1048,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
@@ -1064,273 +1064,273 @@
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B1" s="9" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D1" s="10" t="s">
         <v>1</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>67</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B3" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="C3" s="14" t="s">
         <v>75</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="D3" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="D3" s="14" t="s">
-        <v>77</v>
-      </c>
       <c r="E3" s="14" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D4" s="14" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E4" s="14" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D5" s="14" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E5" s="14" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B6" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="C6" s="14" t="s">
         <v>80</v>
       </c>
-      <c r="C6" s="14" t="s">
-        <v>81</v>
-      </c>
       <c r="D6" s="14" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E6" s="14" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D7" s="14" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E7" s="14" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>56</v>
-      </c>
       <c r="D8" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="D9" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="D9" s="2" t="s">
-        <v>59</v>
-      </c>
       <c r="E9" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B14" s="11"/>
       <c r="C14" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B15" s="1"/>
       <c r="C15" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B16" s="1"/>
       <c r="C16" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>2</v>
@@ -1339,707 +1339,707 @@
         <v>3</v>
       </c>
       <c r="D17" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="E17" s="2" t="s">
         <v>4</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>4</v>
+        <v>97</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>4</v>
+        <v>97</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>4</v>
+        <v>97</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B21" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C21" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C21" s="2" t="s">
-        <v>11</v>
-      </c>
       <c r="D21" s="2" t="s">
-        <v>4</v>
+        <v>97</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>4</v>
+        <v>97</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B23" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C23" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C23" s="2" t="s">
-        <v>14</v>
-      </c>
       <c r="D23" s="2" t="s">
-        <v>4</v>
+        <v>97</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>4</v>
+        <v>97</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B25" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C25" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C25" s="2" t="s">
-        <v>16</v>
-      </c>
       <c r="D25" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="E25" s="2" t="s">
         <v>4</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D26" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="E26" s="2" t="s">
         <v>4</v>
-      </c>
-      <c r="E26" s="2" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D27" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="E27" s="2" t="s">
         <v>4</v>
-      </c>
-      <c r="E27" s="2" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D28" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="E28" s="2" t="s">
         <v>4</v>
-      </c>
-      <c r="E28" s="2" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>4</v>
+        <v>97</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>4</v>
+        <v>97</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>4</v>
+        <v>97</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>4</v>
+        <v>97</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>4</v>
+        <v>97</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>4</v>
+        <v>97</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B35" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C35" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C35" s="2" t="s">
-        <v>26</v>
-      </c>
       <c r="D35" s="2" t="s">
-        <v>4</v>
+        <v>97</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>4</v>
+        <v>97</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>4</v>
+        <v>97</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>4</v>
+        <v>97</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A39" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B39" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C39" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C39" s="2" t="s">
-        <v>31</v>
-      </c>
       <c r="D39" s="2" t="s">
-        <v>4</v>
+        <v>97</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A40" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B40" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C40" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C40" s="2" t="s">
-        <v>33</v>
-      </c>
       <c r="D40" s="2" t="s">
-        <v>4</v>
+        <v>97</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A41" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>4</v>
+        <v>97</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A42" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>4</v>
+        <v>97</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A43" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>4</v>
+        <v>97</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A44" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B44" s="13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C44" s="13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D44" s="13" t="s">
-        <v>4</v>
+        <v>97</v>
       </c>
       <c r="E44" s="13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A45" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B45" s="13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C45" s="13" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D45" s="13" t="s">
-        <v>4</v>
+        <v>97</v>
       </c>
       <c r="E45" s="13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A46" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B46" s="13" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C46" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="D46" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="D46" s="13" t="s">
-        <v>49</v>
-      </c>
       <c r="E46" s="13" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="47" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A47" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B47" s="13" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C47" s="13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D47" s="13" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E47" s="13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="48" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B48" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="C48" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="B48" s="13" t="s">
-        <v>70</v>
-      </c>
-      <c r="C48" s="13" t="s">
-        <v>52</v>
-      </c>
       <c r="D48" s="13" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E48" s="13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="49" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A49" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="50" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A50" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D50" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E50" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="51" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A51" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B51" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C51" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="C51" s="4" t="s">
-        <v>74</v>
-      </c>
       <c r="D51" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E51" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="52" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A52" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B52" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C52" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="C52" s="4" t="s">
+      <c r="D52" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="D52" s="4" t="s">
-        <v>40</v>
-      </c>
       <c r="E52" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="53" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A53" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D53" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E53" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="54" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A54" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="B54" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="B54" s="3" t="s">
-        <v>94</v>
-      </c>
       <c r="C54" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D54" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E54" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="55" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A55" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="B55" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="B55" s="3" t="s">
-        <v>94</v>
-      </c>
       <c r="C55" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D55" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E55" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="56" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A56" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="B56" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="B56" s="3" t="s">
-        <v>94</v>
-      </c>
       <c r="C56" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D56" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E56" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="57" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A57" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="B57" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="B57" s="3" t="s">
-        <v>94</v>
-      </c>
       <c r="C57" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D57" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E57" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="58" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A58" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B58" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C58" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C58" s="2" t="s">
-        <v>47</v>
-      </c>
       <c r="D58" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -2052,6 +2052,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101004D951B9864A79F4AAD2631582B8F2C07" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="6915ecd4dede1209044de4017d7adcfa">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="deb6fef2-38c6-4c24-8b50-885c97b3c555" xmlns:ns3="95d5ab19-5df0-4393-9a78-50cfb5c04389" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c40ca9da527c9bc39f9b86d07e7cfe9e" ns2:_="" ns3:_="">
     <xsd:import namespace="deb6fef2-38c6-4c24-8b50-885c97b3c555"/>
@@ -2262,36 +2277,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5045F2A9-EBCC-4924-AA21-D5DCFB3D44E5}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D3F89562-4375-42AC-80C2-C5E69D9A52EC}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="deb6fef2-38c6-4c24-8b50-885c97b3c555"/>
-    <ds:schemaRef ds:uri="95d5ab19-5df0-4393-9a78-50cfb5c04389"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2314,9 +2303,20 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D3F89562-4375-42AC-80C2-C5E69D9A52EC}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5045F2A9-EBCC-4924-AA21-D5DCFB3D44E5}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="deb6fef2-38c6-4c24-8b50-885c97b3c555"/>
+    <ds:schemaRef ds:uri="95d5ab19-5df0-4393-9a78-50cfb5c04389"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>